<commit_message>
add product import logic
</commit_message>
<xml_diff>
--- a/template/product_template.xlsx
+++ b/template/product_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="11040"/>
+    <workbookView windowHeight="20300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>产品编号</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>备注</t>
+  </si>
+  <si>
+    <t>8000-BW-XLS</t>
+  </si>
+  <si>
+    <t>9x1231.11</t>
+  </si>
+  <si>
+    <t>9000-BW-XLS</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1106,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1164,37 +1173,93 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3">
+        <v>8000</v>
+      </c>
+      <c r="C2" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="E2" s="3">
+        <v>110</v>
+      </c>
+      <c r="F2" s="3">
+        <v>110</v>
+      </c>
+      <c r="G2" s="3">
+        <v>120</v>
+      </c>
+      <c r="H2" s="3">
+        <v>15200</v>
+      </c>
+      <c r="I2" s="3">
+        <v>65.5</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>120</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3">
+        <v>9000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="E3" s="3">
+        <v>110</v>
+      </c>
+      <c r="F3" s="3">
+        <v>110</v>
+      </c>
+      <c r="G3" s="3">
+        <v>120</v>
+      </c>
+      <c r="H3" s="3">
+        <v>15200</v>
+      </c>
+      <c r="I3" s="3">
+        <v>65.5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>120</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15">
@@ -1352,7 +1417,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1 N2:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1 N2 N3 N4:N1048576">
       <formula1>"产品,配件"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>